<commit_message>
Task #2: adapt tests to work as Data Driven test
</commit_message>
<xml_diff>
--- a/testdata/testdata.xlsx
+++ b/testdata/testdata.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sismail30\IdeaProjects\shadow_program\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8A988C-3E1C-44B6-85AE-6945470AA0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D8E30C-3076-4868-99F4-E95A70FAE429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{951FE8B1-BE0C-4DA9-802F-970E48FACD5F}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>password</t>
   </si>
@@ -60,38 +60,19 @@
     <t/>
   </si>
   <si>
-    <t>lTgt3gN@dxc.com</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>qEpjsys@dxc.com</t>
-  </si>
-  <si>
-    <t>g68nPcK@dxc.com</t>
-  </si>
-  <si>
-    <t>b71b1jG@dxc.com</t>
-  </si>
-  <si>
-    <t>LTqYoh7@dxc.com</t>
-  </si>
-  <si>
-    <t>mHdKz6j@dxc.com</t>
-  </si>
-  <si>
-    <t>4p5ZQSH@dxc.com</t>
-  </si>
-  <si>
-    <t>I9SljnO@dxc.com</t>
+    <t>login</t>
+  </si>
+  <si>
+    <t>shimaa1@dxc.com</t>
+  </si>
+  <si>
+    <t>shimaa2@dxc.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -130,12 +111,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -451,90 +431,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0CDA4C8-A7D0-449F-BA2D-639B35454FC6}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.21875"/>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{6B2D1265-2244-4608-A338-25AACB95FA31}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6B2D1265-2244-4608-A338-25AACB95FA31}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{881CEA2D-2CD7-4405-AD3C-F48A7A52EEEB}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{30B288D5-27CD-414E-BB6C-6E243B5EE6EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -548,22 +516,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.88671875"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Task #5: Implement end to end flow
</commit_message>
<xml_diff>
--- a/testdata/testdata.xlsx
+++ b/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sismail30\IdeaProjects\shadow_program\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D8E30C-3076-4868-99F4-E95A70FAE429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A03C2EB-1EC5-400D-8B2D-5B80A018F8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{951FE8B1-BE0C-4DA9-802F-970E48FACD5F}"/>
   </bookViews>
@@ -63,10 +63,10 @@
     <t>login</t>
   </si>
   <si>
-    <t>shimaa1@dxc.com</t>
-  </si>
-  <si>
     <t>shimaa2@dxc.com</t>
+  </si>
+  <si>
+    <t>shimaa3@dxc.com</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0CDA4C8-A7D0-449F-BA2D-639B35454FC6}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>